<commit_message>
Add leaves (but rotations are not right yet)
</commit_message>
<xml_diff>
--- a/mtg_test_geometry.xlsx
+++ b/mtg_test_geometry.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vezy/Documents/cirad/Travail_AMAP/Projets/Cocoa4Future/these_thomas_wibaux/1-tests_mtg/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vezy/Documents/dev/MTG-examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E229882-FEE7-1843-8985-2CBAA5A45328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383484CE-4E3A-704B-ACF9-AFE866E49ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,10 +802,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="3460" topLeftCell="A53" activePane="bottomLeft"/>
-      <selection activeCell="N8" sqref="N8"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64:XFD64"/>
+    <sheetView tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3460" topLeftCell="A37" activePane="bottomLeft"/>
+      <selection activeCell="Q31" sqref="Q31"/>
+      <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1728,7 +1728,7 @@
       </c>
     </row>
     <row r="54" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="F54" s="23" t="s">
+      <c r="E54" s="22" t="s">
         <v>64</v>
       </c>
       <c r="I54" s="8"/>
@@ -1773,7 +1773,7 @@
       </c>
     </row>
     <row r="56" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="F56" s="23" t="s">
+      <c r="E56" s="22" t="s">
         <v>64</v>
       </c>
       <c r="I56" s="8"/>
@@ -1818,7 +1818,7 @@
       </c>
     </row>
     <row r="58" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="F58" s="23" t="s">
+      <c r="E58" s="22" t="s">
         <v>64</v>
       </c>
       <c r="I58" s="8"/>
@@ -1863,7 +1863,7 @@
       </c>
     </row>
     <row r="60" spans="3:17" x14ac:dyDescent="0.2">
-      <c r="F60" s="23" t="s">
+      <c r="E60" s="22" t="s">
         <v>64</v>
       </c>
       <c r="I60" s="8"/>
@@ -1990,21 +1990,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D817E2E441AD8840AD152F485CF91FFD" ma:contentTypeVersion="6" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="66b1d846b1b9efb7ee546c90ee14313c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3bb3ef3-874e-4bfe-a810-81c575a8e62c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f185daa67cb9aaba26ea2e5f6e3f3c05" ns2:_="">
     <xsd:import namespace="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
@@ -2162,10 +2147,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B02E33F-DE6E-4C32-8CFE-5083680231C8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A70317-2E0F-429B-BA37-3DCDF25D9859}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2187,19 +2197,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00A70317-2E0F-429B-BA37-3DCDF25D9859}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B02E33F-DE6E-4C32-8CFE-5083680231C8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="f3bb3ef3-874e-4bfe-a810-81c575a8e62c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix up the leaves orientation (I think I changed the way I measured at this point)
</commit_message>
<xml_diff>
--- a/mtg_test_geometry.xlsx
+++ b/mtg_test_geometry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vezy/Documents/dev/MTG-examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383484CE-4E3A-704B-ACF9-AFE866E49ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C58FA0-0606-BF4A-AABE-52D7E09523F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -802,10 +802,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3460" topLeftCell="A37" activePane="bottomLeft"/>
       <selection activeCell="Q31" sqref="Q31"/>
-      <selection pane="bottomLeft" activeCell="M48" sqref="M48"/>
+      <selection pane="bottomLeft" activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>